<commit_message>
update after requirement chang
-delete admin's permissions in add introduction
-teacher can select a student's homework to check now
-student is able to know how about his homework perform in his class
after teacher checked it now
</commit_message>
<xml_diff>
--- a/doc/API.xlsx
+++ b/doc/API.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="155">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1372,19 +1372,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>data={
-homeworkName : string ,
-homeworkContent : stirng
-totalOfHomeworkSubmit : string ,
-totalOfUngradeHomeworkSubmit : string ,
-studentID : string ,
-studentName : string ,
-srcUrl : string ,
-srcName : string
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">data={
 classList : [{className : string ,
               teacherName : string ,
@@ -1483,6 +1470,9 @@
   </si>
   <si>
     <r>
+      <t>ps:</t>
+    </r>
+    <r>
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
@@ -1490,7 +1480,7 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>去掉</t>
+      <t>所有</t>
     </r>
     <r>
       <rPr>
@@ -1499,7 +1489,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>data</t>
+      <t>string</t>
     </r>
     <r>
       <rPr>
@@ -1509,7 +1499,7 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>中的</t>
+      <t>中的换行符都要换成</t>
     </r>
     <r>
       <rPr>
@@ -1518,11 +1508,9 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>title</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
+      <t xml:space="preserve">&lt;br&gt;
+</t>
+    </r>
     <r>
       <rPr>
         <sz val="12"/>
@@ -1531,7 +1519,7 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>去掉</t>
+      <t>所有和时间有关的</t>
     </r>
     <r>
       <rPr>
@@ -1540,7 +1528,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>postdata</t>
+      <t>string</t>
     </r>
     <r>
       <rPr>
@@ -1550,7 +1538,7 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>中的</t>
+      <t>格式为</t>
     </r>
     <r>
       <rPr>
@@ -1559,89 +1547,6 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>title</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>ps:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>所有</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>string</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>中的换行符都要换成</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">&lt;br&gt;
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>所有和时间有关的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>string</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>格式为</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
       <t>mm/dd/yyyy</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1656,41 +1561,6 @@
         <charset val="134"/>
       </rPr>
       <t>参考资料</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>postdata</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>中</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>srcOfPic</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>变成img</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1903,11 +1773,144 @@
 }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t>if event.type is CHECK, the event.body should contain such words:"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>你本次作业在全班排名前XX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>", whole body should like this:"XX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分，你本次的作业在全班排名前</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>XX"</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data={
+homeworkName : string ,
+homeworkContent : stirng
+totalOfHomeworkSubmit : string ,
+totalOfUngradeHomeworkSubmit : string ,
+studentID : string ,
+studentName : string ,
+srcUrl : string ,
+srcName : string ,
+studentList: [{
+    studentID : string ,
+    studentName : string ,
+    status : string}]
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>postdata={
+userID : string ,
+homeworkID : string ,
+studentID : string
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>update:postdata contains a new element:studentID, it means the data should contain this student's information. And data should contain a list : studentList, which contains all students' id, name and status in this homework.
+Ps:status contains "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>未完成</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>" "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>未评改</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>" "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>已评改</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2344,15 +2347,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="E46" activeCellId="1" sqref="E33 E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="114" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.625" style="5"/>
     <col min="2" max="2" width="22.125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="24" style="4" customWidth="1"/>
+    <col min="3" max="3" width="26.875" style="4" customWidth="1"/>
     <col min="4" max="4" width="56.375" style="4" customWidth="1"/>
     <col min="5" max="5" width="45.625" style="5" customWidth="1"/>
     <col min="6" max="16384" width="20.625" style="5"/>
@@ -2372,7 +2377,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.15">
@@ -2460,9 +2465,6 @@
       <c r="D8" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>124</v>
-      </c>
     </row>
     <row r="9" spans="1:5" ht="114" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
@@ -2494,10 +2496,10 @@
         <v>35</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -2509,13 +2511,10 @@
         <v>34</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="57.95" customHeight="1" x14ac:dyDescent="0.15">
@@ -2534,7 +2533,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>112</v>
@@ -2548,7 +2547,7 @@
         <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>90</v>
@@ -2584,7 +2583,7 @@
         <v>93</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>28</v>
@@ -2592,7 +2591,7 @@
     </row>
     <row r="19" spans="1:5" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>95</v>
@@ -2612,7 +2611,7 @@
         <v>92</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>28</v>
@@ -2640,7 +2639,7 @@
         <v>92</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>28</v>
@@ -2668,7 +2667,7 @@
         <v>92</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>38</v>
@@ -2693,7 +2692,7 @@
         <v>10</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="303.39999999999998" customHeight="1" x14ac:dyDescent="0.15">
@@ -2709,6 +2708,9 @@
       <c r="D27" s="3" t="s">
         <v>113</v>
       </c>
+      <c r="E27" s="5" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="114" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
@@ -2718,7 +2720,7 @@
         <v>12</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>28</v>
@@ -2738,21 +2740,21 @@
         <v>39</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="215.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="114" customHeight="1" x14ac:dyDescent="0.15">
@@ -2777,13 +2779,13 @@
         <v>14</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="198.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="261" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>87</v>
       </c>
@@ -2791,10 +2793,13 @@
         <v>41</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>103</v>
+        <v>153</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>114</v>
+        <v>152</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="156.94999999999999" customHeight="1" x14ac:dyDescent="0.15">
@@ -2805,7 +2810,7 @@
         <v>15</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>106</v>
@@ -2830,7 +2835,7 @@
         <v>10</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="114" customHeight="1" x14ac:dyDescent="0.15">
@@ -2844,7 +2849,7 @@
         <v>107</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="114" customHeight="1" x14ac:dyDescent="0.15">
@@ -2855,7 +2860,7 @@
         <v>17</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>28</v>
@@ -2883,7 +2888,7 @@
         <v>19</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>28</v>
@@ -2897,13 +2902,10 @@
         <v>20</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="114" customHeight="1" x14ac:dyDescent="0.15">
@@ -2914,7 +2916,7 @@
         <v>22</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>28</v>
@@ -2936,24 +2938,24 @@
         <v>23</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="7" customFormat="1" ht="230.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="207.95" customHeight="1" x14ac:dyDescent="0.15">
@@ -2964,24 +2966,24 @@
         <v>24</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="151.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.15">
@@ -3003,7 +3005,7 @@
         <v>10</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="114" customHeight="1" x14ac:dyDescent="0.15">
@@ -3023,7 +3025,7 @@
     <row r="51" spans="1:4" ht="172.15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="52" spans="1:4" ht="114" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>

</xml_diff>